<commit_message>
Chore: Archive legacy DeepSeek scripts and results
</commit_message>
<xml_diff>
--- a/examples/single_agent/analysis/SQ1_Final_Results/sq1_metrics_rules.xlsx
+++ b/examples/single_agent/analysis/SQ1_Final_Results/sq1_metrics_rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Model</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>0|2</t>
+  </si>
+  <si>
+    <t>0|0</t>
   </si>
   <si>
     <t>68|10</t>
@@ -464,7 +467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -754,46 +757,46 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7">
-        <v>728</v>
+        <v>1000</v>
       </c>
       <c r="D7">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="E7">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>78</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>146</v>
+        <v>75</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>24.52</v>
+        <v>39.78</v>
       </c>
       <c r="O7" t="s">
         <v>27</v>
@@ -804,34 +807,34 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8">
-        <v>886</v>
+        <v>728</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="K8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -840,7 +843,7 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>42.24</v>
+        <v>24.52</v>
       </c>
       <c r="O8" t="s">
         <v>28</v>
@@ -851,19 +854,19 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9">
-        <v>897</v>
+        <v>886</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -875,11 +878,11 @@
         <v>0</v>
       </c>
       <c r="J9">
+        <v>9</v>
+      </c>
+      <c r="K9">
         <v>3</v>
       </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
       <c r="L9">
         <v>0</v>
       </c>
@@ -887,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>49.81</v>
+        <v>42.24</v>
       </c>
       <c r="O9" t="s">
         <v>29</v>
@@ -895,37 +898,37 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C10">
-        <v>916</v>
+        <v>897</v>
       </c>
       <c r="D10">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>109</v>
+        <v>3</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -934,10 +937,57 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>27.08</v>
+        <v>49.81</v>
       </c>
       <c r="O10" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>916</v>
+      </c>
+      <c r="D11">
+        <v>24</v>
+      </c>
+      <c r="E11">
+        <v>24</v>
+      </c>
+      <c r="F11">
+        <v>85</v>
+      </c>
+      <c r="G11">
+        <v>85</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>109</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>27.08</v>
+      </c>
+      <c r="O11" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: update Paper3 WRR draft and irrigation metrics spreadsheet
Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/examples/single_agent/analysis/SQ1_Final_Results/sq1_metrics_rules.xlsx
+++ b/examples/single_agent/analysis/SQ1_Final_Results/sq1_metrics_rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
   <si>
     <t>Model</t>
   </si>
@@ -25,24 +25,24 @@
     <t>N</t>
   </si>
   <si>
-    <t>V1_Tot</t>
-  </si>
-  <si>
     <t>V1_Act</t>
   </si>
   <si>
-    <t>V2_Tot</t>
-  </si>
-  <si>
     <t>V2_Act</t>
   </si>
   <si>
-    <t>V3_Tot</t>
-  </si>
-  <si>
     <t>V3_Act</t>
   </si>
   <si>
+    <t>R_H</t>
+  </si>
+  <si>
+    <t>H_norm</t>
+  </si>
+  <si>
+    <t>EBE</t>
+  </si>
+  <si>
     <t>Intv</t>
   </si>
   <si>
@@ -52,9 +52,6 @@
     <t>Intv_P</t>
   </si>
   <si>
-    <t>Intv_H</t>
-  </si>
-  <si>
     <t>FF</t>
   </si>
   <si>
@@ -70,6 +67,15 @@
     <t>gemma3_27b</t>
   </si>
   <si>
+    <t>ministral3_3b</t>
+  </si>
+  <si>
+    <t>ministral3_8b</t>
+  </si>
+  <si>
+    <t>ministral3_14b</t>
+  </si>
+  <si>
     <t>Group_A</t>
   </si>
   <si>
@@ -82,19 +88,55 @@
     <t>1|0</t>
   </si>
   <si>
-    <t>1|32</t>
-  </si>
-  <si>
-    <t>0|43</t>
+    <t>4|28</t>
+  </si>
+  <si>
+    <t>4|36</t>
   </si>
   <si>
     <t>0|1</t>
   </si>
   <si>
-    <t>2|4</t>
+    <t>30|5</t>
+  </si>
+  <si>
+    <t>8|1</t>
   </si>
   <si>
     <t>0|0</t>
+  </si>
+  <si>
+    <t>5|0</t>
+  </si>
+  <si>
+    <t>2|1</t>
+  </si>
+  <si>
+    <t>1|1</t>
+  </si>
+  <si>
+    <t>33|44</t>
+  </si>
+  <si>
+    <t>29|32</t>
+  </si>
+  <si>
+    <t>7|0</t>
+  </si>
+  <si>
+    <t>10|4</t>
+  </si>
+  <si>
+    <t>17|29</t>
+  </si>
+  <si>
+    <t>2|3</t>
+  </si>
+  <si>
+    <t>12|15</t>
+  </si>
+  <si>
+    <t>8|14</t>
   </si>
 </sst>
 </file>
@@ -452,13 +494,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,16 +543,13 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>998</v>
@@ -519,22 +558,22 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="F2">
-        <v>36</v>
+        <v>171</v>
       </c>
       <c r="G2">
-        <v>36</v>
+        <v>20.84</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.6637999999999999</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.5255</v>
       </c>
       <c r="J2">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -543,115 +582,106 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
         <v>14.14</v>
       </c>
-      <c r="O2" t="s">
+      <c r="N2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" t="s">
+      <c r="C3">
+        <v>855</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>0.58</v>
+      </c>
+      <c r="H3">
+        <v>0.7897</v>
+      </c>
+      <c r="I3">
+        <v>0.7851</v>
+      </c>
+      <c r="J3">
+        <v>245</v>
+      </c>
+      <c r="K3">
+        <v>103</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>46.36</v>
+      </c>
+      <c r="N3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>857</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>2.8</v>
+      </c>
+      <c r="H4">
+        <v>0.8043</v>
+      </c>
+      <c r="I4">
+        <v>0.7818000000000001</v>
+      </c>
+      <c r="J4">
+        <v>336</v>
+      </c>
+      <c r="K4">
+        <v>123</v>
+      </c>
+      <c r="L4">
+        <v>21</v>
+      </c>
+      <c r="M4">
+        <v>49.01</v>
+      </c>
+      <c r="N4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3">
-        <v>827</v>
-      </c>
-      <c r="D3">
-        <v>42</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>99</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>141</v>
-      </c>
-      <c r="K3">
-        <v>42</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>39.61</v>
-      </c>
-      <c r="O3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>20</v>
-      </c>
-      <c r="C4">
-        <v>843</v>
-      </c>
-      <c r="D4">
-        <v>53</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>115</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>168</v>
-      </c>
-      <c r="K4">
-        <v>53</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>37.42</v>
-      </c>
-      <c r="O4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
       </c>
       <c r="C5">
         <v>999</v>
@@ -660,22 +690,22 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="F5">
-        <v>89</v>
+        <v>8</v>
       </c>
       <c r="G5">
-        <v>89</v>
+        <v>9.710000000000001</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>0.4713</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>0.4255</v>
       </c>
       <c r="J5">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -684,107 +714,626 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
         <v>17.58</v>
       </c>
-      <c r="O5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="N5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>883</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0.4781</v>
+      </c>
+      <c r="I6">
+        <v>0.4781</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>32.69</v>
+      </c>
+      <c r="N6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>962</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0.4728</v>
+      </c>
+      <c r="I7">
+        <v>0.4728</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7">
+        <v>33.41</v>
+      </c>
+      <c r="N7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>1000</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>18</v>
+      </c>
+      <c r="F8">
+        <v>69</v>
+      </c>
+      <c r="G8">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="H8">
+        <v>0.6955</v>
+      </c>
+      <c r="I8">
+        <v>0.635</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>32.67</v>
+      </c>
+      <c r="N8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>984</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0.629</v>
+      </c>
+      <c r="I9">
+        <v>0.629</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>46.15</v>
+      </c>
+      <c r="N9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>997</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0.6848</v>
+      </c>
+      <c r="I10">
+        <v>0.6848</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>52.29</v>
+      </c>
+      <c r="N10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>991</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>84</v>
+      </c>
+      <c r="F11">
+        <v>52</v>
+      </c>
+      <c r="G11">
+        <v>13.82</v>
+      </c>
+      <c r="H11">
+        <v>0.4355</v>
+      </c>
+      <c r="I11">
+        <v>0.3753</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>10.1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>688</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1.45</v>
+      </c>
+      <c r="H12">
+        <v>0.755</v>
+      </c>
+      <c r="I12">
+        <v>0.7441</v>
+      </c>
+      <c r="J12">
+        <v>217</v>
+      </c>
+      <c r="K12">
+        <v>102</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <v>54.53</v>
+      </c>
+      <c r="N12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13">
+        <v>764</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0.13</v>
+      </c>
+      <c r="H13">
+        <v>0.6401</v>
+      </c>
+      <c r="I13">
+        <v>0.6393</v>
+      </c>
+      <c r="J13">
+        <v>202</v>
+      </c>
+      <c r="K13">
+        <v>102</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <v>42.77</v>
+      </c>
+      <c r="N13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>984</v>
+      </c>
+      <c r="D14">
+        <v>7</v>
+      </c>
+      <c r="E14">
+        <v>31</v>
+      </c>
+      <c r="F14">
+        <v>80</v>
+      </c>
+      <c r="G14">
+        <v>11.99</v>
+      </c>
+      <c r="H14">
+        <v>0.7524999999999999</v>
+      </c>
+      <c r="I14">
+        <v>0.6623</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>18.55</v>
+      </c>
+      <c r="N14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>948</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0.6269</v>
+      </c>
+      <c r="I15">
+        <v>0.6269</v>
+      </c>
+      <c r="J15">
+        <v>167</v>
+      </c>
+      <c r="K15">
+        <v>97</v>
+      </c>
+      <c r="L15">
+        <v>8</v>
+      </c>
+      <c r="M15">
+        <v>43.63</v>
+      </c>
+      <c r="N15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>816</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0.6292</v>
+      </c>
+      <c r="I16">
+        <v>0.6292</v>
+      </c>
+      <c r="J16">
+        <v>100</v>
+      </c>
+      <c r="K16">
+        <v>57</v>
+      </c>
+      <c r="L16">
+        <v>23</v>
+      </c>
+      <c r="M16">
+        <v>40.34</v>
+      </c>
+      <c r="N16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="C6">
-        <v>969</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>973</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>91</v>
+      </c>
+      <c r="F17">
+        <v>20</v>
+      </c>
+      <c r="G17">
+        <v>11.61</v>
+      </c>
+      <c r="H17">
+        <v>0.4805</v>
+      </c>
+      <c r="I17">
+        <v>0.4247</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>16.95</v>
+      </c>
+      <c r="N17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>889</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0.6951000000000001</v>
+      </c>
+      <c r="I18">
+        <v>0.6951000000000001</v>
+      </c>
+      <c r="J18">
+        <v>97</v>
+      </c>
+      <c r="K18">
+        <v>52</v>
+      </c>
+      <c r="L18">
+        <v>3</v>
+      </c>
+      <c r="M18">
+        <v>55.01</v>
+      </c>
+      <c r="N18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>32</v>
-      </c>
-      <c r="K6">
-        <v>10</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>24.86</v>
-      </c>
-      <c r="O6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7">
-        <v>1000</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>18</v>
-      </c>
-      <c r="G7">
-        <v>18</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>18</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>32.67</v>
-      </c>
-      <c r="O7" t="s">
-        <v>26</v>
+      <c r="C19">
+        <v>927</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0.7125</v>
+      </c>
+      <c r="I19">
+        <v>0.7125</v>
+      </c>
+      <c r="J19">
+        <v>148</v>
+      </c>
+      <c r="K19">
+        <v>83</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>51.51</v>
+      </c>
+      <c r="N19" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>